<commit_message>
pulling from remote and adding JUnit tests
</commit_message>
<xml_diff>
--- a/Scrum_elements/Product Backlog.xlsx
+++ b/Scrum_elements/Product Backlog.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="125">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -398,12 +398,6 @@
   </si>
   <si>
     <t>(blank)</t>
-  </si>
-  <si>
-    <t>(Offline test) 34</t>
-  </si>
-  <si>
-    <t>(Done up to this) 38</t>
   </si>
 </sst>
 </file>
@@ -1287,7 +1281,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -1767,8 +1761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2376,8 +2370,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>125</v>
+      <c r="A36">
+        <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>50</v>
@@ -2444,8 +2438,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>126</v>
+      <c r="A40">
+        <v>38</v>
       </c>
       <c r="B40" t="s">
         <v>66</v>

</xml_diff>